<commit_message>
logo and clean pages
</commit_message>
<xml_diff>
--- a/data/sales.xlsx
+++ b/data/sales.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eliottlegendre/Documents/prive/Footsteps/footsteps/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55E2868-590A-3C4D-9A77-7D8EC60961AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEF8D3D-F571-2946-A0F6-B1A51DB9074E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15460" xr2:uid="{CBF956DE-54A9-734E-90A0-7EF75042D42E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Nom</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Danny</t>
   </si>
   <si>
-    <t>2 prima, 1 mix, 1 equilux 1 pumpkin</t>
-  </si>
-  <si>
     <t>Cat</t>
   </si>
   <si>
@@ -116,22 +113,31 @@
     <t>Paco</t>
   </si>
   <si>
-    <t>1 san marco, 1 antico, 5 SanMarco</t>
-  </si>
-  <si>
     <t>Benoit</t>
   </si>
   <si>
-    <t>1 equilux, 5 SanMarco</t>
-  </si>
-  <si>
     <t>Clem</t>
   </si>
   <si>
-    <t>1 prima, 1 antico, 5 SanMarco</t>
-  </si>
-  <si>
-    <t>1 prima, 4 decouvertes, 4 packs 6</t>
+    <t>1 prima, 4 decouvertes, 4 packs 6, 4</t>
+  </si>
+  <si>
+    <t>2 prima, 1 mix, 1 equilux, 1 pumpkin, 3 smarco, 2 ss, 1 chipmunk</t>
+  </si>
+  <si>
+    <t>1 san marco, 1 antico, 5 smarco</t>
+  </si>
+  <si>
+    <t>1 equilux, 5 smarco</t>
+  </si>
+  <si>
+    <t>Theo B</t>
+  </si>
+  <si>
+    <t>1 equilux, 1 antico</t>
+  </si>
+  <si>
+    <t>1 prima, 1 antico, 5 smarco</t>
   </si>
 </sst>
 </file>
@@ -487,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC98B898-7ED1-EA43-80FD-DE7ABC346C2D}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,7 +523,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1">
         <v>78</v>
@@ -528,18 +534,18 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
       <c r="D4" s="1">
         <v>10</v>
@@ -550,10 +556,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
       </c>
       <c r="D5" s="1">
         <v>8</v>
@@ -561,25 +567,25 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
       </c>
       <c r="D9" s="1">
         <v>40</v>
@@ -587,10 +593,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
         <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
       </c>
       <c r="D10" s="1">
         <v>14</v>
@@ -598,10 +604,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
         <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
       </c>
       <c r="D11" s="1">
         <v>24</v>
@@ -609,10 +615,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
         <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
       </c>
       <c r="D12" s="1">
         <v>18</v>
@@ -620,10 +626,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
         <v>23</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
       </c>
       <c r="D13" s="1">
         <v>46</v>
@@ -634,10 +640,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D14" s="1">
         <v>52</v>
@@ -648,10 +654,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1">
         <v>6</v>
@@ -659,12 +665,23 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="1">
         <v>51</v>
       </c>
     </row>

</xml_diff>